<commit_message>
static historical sim and analysis
</commit_message>
<xml_diff>
--- a/historical-dyn-swr-sim.xlsx
+++ b/historical-dyn-swr-sim.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/monte-carlo-simulation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F5F5FD-86A1-4D4F-B96A-E15AA60E8439}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F0D163-9FBF-AA44-96AC-712CD3500050}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="1460" windowWidth="24640" windowHeight="13680" activeTab="1" xr2:uid="{C1D6D8DA-D5CE-A94C-BE1E-5C565E50FC3F}"/>
+    <workbookView xWindow="240" yWindow="2060" windowWidth="24640" windowHeight="13680" xr2:uid="{C1D6D8DA-D5CE-A94C-BE1E-5C565E50FC3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18751,7 +18751,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865000FF-6F65-FF45-871E-2851010916C8}">
   <dimension ref="A1:AY87"/>
   <sheetViews>
-    <sheetView topLeftCell="AU40" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AO42" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AX48" sqref="A48:AX87"/>
     </sheetView>
   </sheetViews>
@@ -31085,7 +31085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E56E9E4-BACF-1347-9878-B204AA69AA8C}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="B10" workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D51"/>
     </sheetView>
   </sheetViews>

</xml_diff>